<commit_message>
giving up for tonight
</commit_message>
<xml_diff>
--- a/data-dictionary/Dictionary.ACO.SSP.COUNTY.ASSIGNED.PUF.2018.xlsx
+++ b/data-dictionary/Dictionary.ACO.SSP.COUNTY.ASSIGNED.PUF.2018.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\DAFDA\Website Updates\PY 2018 County Assigned PUF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/karenjiang/Documents/Gov 1005 Data/Final-Project/data-dictionary/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FF33588-74DB-9B46-A613-FD272C00EB64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="14460" yWindow="460" windowWidth="11140" windowHeight="15540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="File Layout" sheetId="1" r:id="rId1"/>
@@ -321,7 +322,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -568,8 +569,8 @@
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2 2" xfId="1"/>
-    <cellStyle name="Normal 3" xfId="2"/>
+    <cellStyle name="Normal 2 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -846,28 +847,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:LS2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:331" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>
@@ -1018,7 +1019,7 @@
       <c r="LR1" s="1"/>
       <c r="LS1" s="1"/>
     </row>
-    <row r="2" spans="1:331" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:331" x14ac:dyDescent="0.2">
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1351,20 +1352,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="26" customWidth="1"/>
+    <col min="1" max="1" width="22.5" style="26" customWidth="1"/>
     <col min="2" max="2" width="21" style="26" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="54.28515625" style="26" customWidth="1"/>
-    <col min="4" max="4" width="45.42578125" style="26" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="26"/>
+    <col min="3" max="3" width="54.33203125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="45.5" style="26" customWidth="1"/>
+    <col min="5" max="16384" width="9.1640625" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1395,7 +1396,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A3" s="27" t="s">
         <v>19</v>
       </c>
@@ -1409,7 +1410,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="27" t="s">
         <v>27</v>
       </c>
@@ -1423,7 +1424,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="27" t="s">
         <v>28</v>
       </c>
@@ -1437,7 +1438,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="27" t="s">
         <v>29</v>
       </c>
@@ -1451,7 +1452,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A7" s="27" t="s">
         <v>30</v>
       </c>
@@ -1465,7 +1466,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="30" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="30" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A8" s="27" t="s">
         <v>31</v>
       </c>
@@ -1479,7 +1480,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="30" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="30" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A9" s="27" t="s">
         <v>32</v>
       </c>
@@ -1493,7 +1494,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="30" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="30" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A10" s="27" t="s">
         <v>33</v>
       </c>
@@ -1507,7 +1508,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="30" customFormat="1" ht="89.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" s="30" customFormat="1" ht="105" x14ac:dyDescent="0.2">
       <c r="A11" s="27" t="s">
         <v>34</v>
       </c>
@@ -1521,7 +1522,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="12" spans="1:4" s="30" customFormat="1" ht="51" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" s="27" t="s">
         <v>35</v>
       </c>
@@ -1535,7 +1536,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="51" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" s="27" t="s">
         <v>36</v>
       </c>
@@ -1556,23 +1557,23 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:X64"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="26"/>
-    <col min="2" max="2" width="34.28515625" style="26" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" style="26" customWidth="1"/>
-    <col min="4" max="4" width="44.5703125" style="26" customWidth="1"/>
-    <col min="5" max="5" width="39.5703125" style="26" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" style="26" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" style="26" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="26"/>
+    <col min="1" max="1" width="9.1640625" style="26"/>
+    <col min="2" max="2" width="34.33203125" style="26" customWidth="1"/>
+    <col min="3" max="3" width="15.83203125" style="26" customWidth="1"/>
+    <col min="4" max="4" width="44.5" style="26" customWidth="1"/>
+    <col min="5" max="5" width="39.5" style="26" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" style="26" customWidth="1"/>
+    <col min="7" max="7" width="14.1640625" style="26" customWidth="1"/>
+    <col min="8" max="16384" width="9.1640625" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
@@ -1604,7 +1605,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:14" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="30" x14ac:dyDescent="0.2">
       <c r="A4" s="33">
         <v>2018</v>
       </c>
@@ -2531,7 +2532,7 @@
     <mergeCell ref="A22:C22"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A7" r:id="rId1" display="https://www.cms.gov/Medicare/Medicare-Fee-for-Service-Payment/sharedsavingsprogram/Downloads/ACO-ID-crosswalk.xlsx"/>
+    <hyperlink ref="A7" r:id="rId1" display="https://www.cms.gov/Medicare/Medicare-Fee-for-Service-Payment/sharedsavingsprogram/Downloads/ACO-ID-crosswalk.xlsx" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
@@ -2539,6 +2540,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <Calendar_x0020_Year xmlns="81d1232f-70db-4e1b-9853-8d9bb280f40b">2018</Calendar_x0020_Year>
@@ -2553,21 +2563,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="86a8e296-5f29-4af2-954b-0de0d1e1f8bc" ContentTypeId="0x0101" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010016E175D1D4D77C40853E837E21916AC7" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f1642a185fd361a6e53b2a0824d299fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81d1232f-70db-4e1b-9853-8d9bb280f40b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3c63b68726d54b62a6c355afdbf16112" ns2:_="">
     <xsd:import namespace="81d1232f-70db-4e1b-9853-8d9bb280f40b"/>
@@ -2811,7 +2807,20 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="86a8e296-5f29-4af2-954b-0de0d1e1f8bc" ContentTypeId="0x0101" PreviousValue="false"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{347110E6-0E6F-4C13-AE46-5796328ADA52}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4E47DC75-26E2-4B7A-A229-A08BE79F7184}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -2827,23 +2836,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{347110E6-0E6F-4C13-AE46-5796328ADA52}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A87E3DE1-706B-4FFD-BE1F-496F5BD50009}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0682086C-F4D1-4DFF-BC8B-9A235AA79521}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2859,4 +2852,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A87E3DE1-706B-4FFD-BE1F-496F5BD50009}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>